<commit_message>
Add G_GET_RSSI instruction for host and robot; revise XBee API send/receive/parse organization
</commit_message>
<xml_diff>
--- a/Host/XBee-Host_Communication.xlsx
+++ b/Host/XBee-Host_Communication.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jared/Documents/SWEP/SWEP-2019/Host/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172964BC-2321-DC46-9816-EFC86AD856B4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BE9145-AA4E-834B-BAE7-036E3AC0CF47}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{D18BBAC1-CF6A-294C-87FD-DCA6CF7D8B74}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" activeTab="1" xr2:uid="{D18BBAC1-CF6A-294C-87FD-DCA6CF7D8B74}"/>
   </bookViews>
   <sheets>
     <sheet name="HostSingle" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="101">
   <si>
     <t>B1 (INS)</t>
   </si>
@@ -308,6 +308,33 @@
   </si>
   <si>
     <t>SET_POS*</t>
+  </si>
+  <si>
+    <t>GET_RSSI</t>
+  </si>
+  <si>
+    <t>startRssi()</t>
+  </si>
+  <si>
+    <t>This initiates the arduino to halt all movement and record the RSSI values for n beacons. Upon receiving the last beacon pulse, the arduino will send a repsonse to the host with the observed RSSI values</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>Variable length response containing reported RSSI values from the bot</t>
+  </si>
+  <si>
+    <t>Gets the RSSI values from the indicated number of beacons, not including the main Xbee beacon</t>
+  </si>
+  <si>
+    <t>RESERVED</t>
+  </si>
+  <si>
+    <t>nextBeacon()</t>
+  </si>
+  <si>
+    <t>Additional ping from beacons. Uint8 is the beacon's ID number</t>
   </si>
 </sst>
 </file>
@@ -677,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CB75C70-85E8-1B4D-8509-2B395374D93A}">
   <dimension ref="A4:X261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="L140" sqref="L140:O140"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -689,7 +716,7 @@
     <col min="8" max="9" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="12" width="3.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="15" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="51" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="20" width="3.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="23" width="4.33203125" bestFit="1" customWidth="1"/>
@@ -921,9 +948,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
@@ -932,10 +959,22 @@
       <c r="C15">
         <v>9</v>
       </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>93</v>
+      </c>
+      <c r="X15" s="2" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>98</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
@@ -943,6 +982,15 @@
       </c>
       <c r="C16">
         <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+      <c r="P16" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -3996,17 +4044,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1F5E4D-12FB-C749-8B73-7BB9522DEC8B}">
-  <dimension ref="A4:AC12"/>
+  <dimension ref="A4:AC13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="9" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="18" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="18" width="3.33203125" bestFit="1" customWidth="1"/>
     <col min="19" max="27" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="46.1640625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="30.1640625" bestFit="1" customWidth="1"/>
@@ -4223,6 +4272,29 @@
       <c r="Z12" s="4"/>
       <c r="AB12" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>92</v>
+      </c>
+      <c r="J13" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" t="s">
+        <v>19</v>
+      </c>
+      <c r="M13" t="s">
+        <v>19</v>
+      </c>
+      <c r="N13" t="s">
+        <v>95</v>
+      </c>
+      <c r="AB13" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add arduino and host code for entire system under PID controller
</commit_message>
<xml_diff>
--- a/Host/XBee-Host_Communication.xlsx
+++ b/Host/XBee-Host_Communication.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jared/Documents/SWEP/SWEP-2019/Host/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4BE9145-AA4E-834B-BAE7-036E3AC0CF47}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793AB9C2-0C02-2F45-A4C3-C031DC8310D5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" activeTab="1" xr2:uid="{D18BBAC1-CF6A-294C-87FD-DCA6CF7D8B74}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{D18BBAC1-CF6A-294C-87FD-DCA6CF7D8B74}"/>
   </bookViews>
   <sheets>
     <sheet name="HostSingle" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="99">
   <si>
     <t>B1 (INS)</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Mnemonic</t>
   </si>
   <si>
-    <t>GO</t>
-  </si>
-  <si>
     <t>GET_X</t>
   </si>
   <si>
@@ -70,9 +67,6 @@
     <t>DEC</t>
   </si>
   <si>
-    <t>GO_F</t>
-  </si>
-  <si>
     <t>unused</t>
   </si>
   <si>
@@ -130,12 +124,6 @@
     <t>Function called</t>
   </si>
   <si>
-    <t>Tells bot to move</t>
-  </si>
-  <si>
-    <t>go()</t>
-  </si>
-  <si>
     <t>Get bot's x coordinate</t>
   </si>
   <si>
@@ -169,36 +157,18 @@
     <t>getBattery()</t>
   </si>
   <si>
-    <t>Tells bot to stop</t>
-  </si>
-  <si>
-    <t>dontGo()</t>
-  </si>
-  <si>
     <t>Sets a bot's x</t>
   </si>
   <si>
     <t>Sets a bot's y</t>
   </si>
   <si>
-    <t>Sets a bot's right motor</t>
-  </si>
-  <si>
-    <t>Sets a bot's left motor</t>
-  </si>
-  <si>
-    <t>Tells a bot to move for a fixed duration in milliseconds</t>
-  </si>
-  <si>
     <t>Sets a bot's x, y, and theta</t>
   </si>
   <si>
     <t>getPos()</t>
   </si>
   <si>
-    <t>goFixed()</t>
-  </si>
-  <si>
     <t>setX()</t>
   </si>
   <si>
@@ -208,12 +178,6 @@
     <t>setAngle()</t>
   </si>
   <si>
-    <t>setLeftMotor()</t>
-  </si>
-  <si>
-    <t>setRightMotor()</t>
-  </si>
-  <si>
     <t>setPos()</t>
   </si>
   <si>
@@ -277,9 +241,6 @@
     <t>B17</t>
   </si>
   <si>
-    <t>int16</t>
-  </si>
-  <si>
     <t>GET_B*</t>
   </si>
   <si>
@@ -301,12 +262,6 @@
     <t>SET_A*</t>
   </si>
   <si>
-    <t>SET_M_L*</t>
-  </si>
-  <si>
-    <t>SET_M_R*</t>
-  </si>
-  <si>
     <t>SET_POS*</t>
   </si>
   <si>
@@ -335,6 +290,45 @@
   </si>
   <si>
     <t>Additional ping from beacons. Uint8 is the beacon's ID number</t>
+  </si>
+  <si>
+    <t>Used to be GO</t>
+  </si>
+  <si>
+    <t>Tells bot the program is done</t>
+  </si>
+  <si>
+    <t>done()</t>
+  </si>
+  <si>
+    <t>Used to be GO_F</t>
+  </si>
+  <si>
+    <t>GET_NEXT</t>
+  </si>
+  <si>
+    <t>Asks host for the next point to navigate to</t>
+  </si>
+  <si>
+    <t>Used to be SET_M_L</t>
+  </si>
+  <si>
+    <t>Used to be SET_M_R</t>
+  </si>
+  <si>
+    <t>nextTarget()</t>
+  </si>
+  <si>
+    <t>Response to a bot's request for next target point</t>
+  </si>
+  <si>
+    <t>START_LOCAL</t>
+  </si>
+  <si>
+    <t>Response indicating localized x and y of a bot</t>
+  </si>
+  <si>
+    <t>endLocalization()</t>
   </si>
 </sst>
 </file>
@@ -704,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CB75C70-85E8-1B4D-8509-2B395374D93A}">
   <dimension ref="A4:X261"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -733,80 +727,70 @@
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="I4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" s="1" t="s">
+      <c r="P4" t="s">
         <v>28</v>
       </c>
-      <c r="P4" t="s">
-        <v>30</v>
-      </c>
       <c r="Q4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="X4" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="str">
-        <f>DEC2HEX(C6)</f>
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="P6" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" ref="B7:B70" si="0">DEC2HEX(C7)</f>
@@ -816,15 +800,15 @@
         <v>1</v>
       </c>
       <c r="P7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="Q7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
@@ -834,15 +818,15 @@
         <v>2</v>
       </c>
       <c r="P8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Q8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
@@ -852,15 +836,15 @@
         <v>3</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="Q9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
@@ -870,15 +854,15 @@
         <v>4</v>
       </c>
       <c r="P10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="Q10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
@@ -888,15 +872,15 @@
         <v>5</v>
       </c>
       <c r="P11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="Q11" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
@@ -906,15 +890,15 @@
         <v>6</v>
       </c>
       <c r="P12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="Q12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
@@ -924,15 +908,15 @@
         <v>7</v>
       </c>
       <c r="P13" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="Q13" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
@@ -942,15 +926,15 @@
         <v>8</v>
       </c>
       <c r="P14" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="Q14" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:24" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
@@ -960,21 +944,21 @@
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="Q15" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="X15" s="2" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
@@ -984,18 +968,18 @@
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P16" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="Q16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>90</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
@@ -1004,10 +988,28 @@
       <c r="C17">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="P17" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
@@ -1016,10 +1018,28 @@
       <c r="C18">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="P18" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
@@ -1029,9 +1049,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
@@ -1041,9 +1061,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
@@ -1053,9 +1073,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
@@ -1065,9 +1085,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
@@ -1077,9 +1097,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="0"/>
@@ -1089,9 +1109,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
@@ -1101,9 +1121,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
@@ -1113,9 +1133,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B27" t="str">
         <f t="shared" si="0"/>
@@ -1125,9 +1145,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="0"/>
@@ -1137,9 +1157,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B29" t="str">
         <f t="shared" si="0"/>
@@ -1149,9 +1169,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
@@ -1161,9 +1181,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B31" t="str">
         <f t="shared" si="0"/>
@@ -1173,9 +1193,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B32" t="str">
         <f t="shared" si="0"/>
@@ -1187,7 +1207,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" si="0"/>
@@ -1199,7 +1219,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" si="0"/>
@@ -1211,7 +1231,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
@@ -1223,7 +1243,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
@@ -1235,7 +1255,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
@@ -1247,7 +1267,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
@@ -1259,7 +1279,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
@@ -1271,7 +1291,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="0"/>
@@ -1283,7 +1303,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="0"/>
@@ -1295,7 +1315,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
@@ -1307,7 +1327,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B43" t="str">
         <f t="shared" si="0"/>
@@ -1319,7 +1339,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B44" t="str">
         <f t="shared" si="0"/>
@@ -1331,7 +1351,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
@@ -1343,7 +1363,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
@@ -1355,7 +1375,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B47" t="str">
         <f t="shared" si="0"/>
@@ -1367,7 +1387,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B48" t="str">
         <f t="shared" si="0"/>
@@ -1379,7 +1399,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B49" t="str">
         <f t="shared" si="0"/>
@@ -1391,7 +1411,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B50" t="str">
         <f t="shared" si="0"/>
@@ -1403,7 +1423,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" si="0"/>
@@ -1415,7 +1435,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B52" t="str">
         <f t="shared" si="0"/>
@@ -1427,7 +1447,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B53" t="str">
         <f t="shared" si="0"/>
@@ -1439,7 +1459,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B54" t="str">
         <f t="shared" si="0"/>
@@ -1451,7 +1471,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B55" t="str">
         <f t="shared" si="0"/>
@@ -1463,7 +1483,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B56" t="str">
         <f t="shared" si="0"/>
@@ -1475,7 +1495,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B57" t="str">
         <f t="shared" si="0"/>
@@ -1487,7 +1507,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B58" t="str">
         <f t="shared" si="0"/>
@@ -1499,7 +1519,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B59" t="str">
         <f t="shared" si="0"/>
@@ -1511,7 +1531,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B60" t="str">
         <f t="shared" si="0"/>
@@ -1523,7 +1543,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B61" t="str">
         <f t="shared" si="0"/>
@@ -1535,7 +1555,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B62" t="str">
         <f t="shared" si="0"/>
@@ -1547,7 +1567,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B63" t="str">
         <f t="shared" si="0"/>
@@ -1559,7 +1579,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B64" t="str">
         <f t="shared" si="0"/>
@@ -1571,7 +1591,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B65" t="str">
         <f t="shared" si="0"/>
@@ -1583,7 +1603,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B66" t="str">
         <f t="shared" si="0"/>
@@ -1595,7 +1615,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B67" t="str">
         <f t="shared" si="0"/>
@@ -1607,7 +1627,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B68" t="str">
         <f t="shared" si="0"/>
@@ -1619,7 +1639,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B69" t="str">
         <f t="shared" si="0"/>
@@ -1631,7 +1651,7 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B70" t="str">
         <f t="shared" si="0"/>
@@ -1643,7 +1663,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B71" t="str">
         <f t="shared" ref="B71:B134" si="1">DEC2HEX(C71)</f>
@@ -1655,7 +1675,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B72" t="str">
         <f t="shared" si="1"/>
@@ -1667,7 +1687,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B73" t="str">
         <f t="shared" si="1"/>
@@ -1679,7 +1699,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B74" t="str">
         <f t="shared" si="1"/>
@@ -1691,7 +1711,7 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B75" t="str">
         <f t="shared" si="1"/>
@@ -1703,7 +1723,7 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B76" t="str">
         <f t="shared" si="1"/>
@@ -1715,7 +1735,7 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B77" t="str">
         <f t="shared" si="1"/>
@@ -1727,7 +1747,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B78" t="str">
         <f t="shared" si="1"/>
@@ -1739,7 +1759,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B79" t="str">
         <f t="shared" si="1"/>
@@ -1751,7 +1771,7 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B80" t="str">
         <f t="shared" si="1"/>
@@ -1763,7 +1783,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B81" t="str">
         <f t="shared" si="1"/>
@@ -1775,7 +1795,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B82" t="str">
         <f t="shared" si="1"/>
@@ -1787,7 +1807,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B83" t="str">
         <f t="shared" si="1"/>
@@ -1799,7 +1819,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B84" t="str">
         <f t="shared" si="1"/>
@@ -1811,7 +1831,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B85" t="str">
         <f t="shared" si="1"/>
@@ -1823,7 +1843,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B86" t="str">
         <f t="shared" si="1"/>
@@ -1835,7 +1855,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B87" t="str">
         <f t="shared" si="1"/>
@@ -1847,7 +1867,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B88" t="str">
         <f t="shared" si="1"/>
@@ -1859,7 +1879,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B89" t="str">
         <f t="shared" si="1"/>
@@ -1871,7 +1891,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B90" t="str">
         <f t="shared" si="1"/>
@@ -1883,7 +1903,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B91" t="str">
         <f t="shared" si="1"/>
@@ -1895,7 +1915,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B92" t="str">
         <f t="shared" si="1"/>
@@ -1907,7 +1927,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B93" t="str">
         <f t="shared" si="1"/>
@@ -1919,7 +1939,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B94" t="str">
         <f t="shared" si="1"/>
@@ -1931,7 +1951,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B95" t="str">
         <f t="shared" si="1"/>
@@ -1943,7 +1963,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B96" t="str">
         <f t="shared" si="1"/>
@@ -1955,7 +1975,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B97" t="str">
         <f t="shared" si="1"/>
@@ -1967,7 +1987,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B98" t="str">
         <f t="shared" si="1"/>
@@ -1979,7 +1999,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B99" t="str">
         <f t="shared" si="1"/>
@@ -1991,7 +2011,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B100" t="str">
         <f t="shared" si="1"/>
@@ -2003,7 +2023,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B101" t="str">
         <f t="shared" si="1"/>
@@ -2015,7 +2035,7 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B102" t="str">
         <f t="shared" si="1"/>
@@ -2027,7 +2047,7 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B103" t="str">
         <f t="shared" si="1"/>
@@ -2039,7 +2059,7 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B104" t="str">
         <f t="shared" si="1"/>
@@ -2051,7 +2071,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B105" t="str">
         <f t="shared" si="1"/>
@@ -2063,7 +2083,7 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B106" t="str">
         <f t="shared" si="1"/>
@@ -2075,7 +2095,7 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B107" t="str">
         <f t="shared" si="1"/>
@@ -2087,7 +2107,7 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B108" t="str">
         <f t="shared" si="1"/>
@@ -2099,7 +2119,7 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B109" t="str">
         <f t="shared" si="1"/>
@@ -2111,7 +2131,7 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B110" t="str">
         <f t="shared" si="1"/>
@@ -2123,7 +2143,7 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B111" t="str">
         <f t="shared" si="1"/>
@@ -2135,7 +2155,7 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B112" t="str">
         <f t="shared" si="1"/>
@@ -2147,7 +2167,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B113" t="str">
         <f t="shared" si="1"/>
@@ -2159,7 +2179,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B114" t="str">
         <f t="shared" si="1"/>
@@ -2171,7 +2191,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B115" t="str">
         <f t="shared" si="1"/>
@@ -2183,7 +2203,7 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B116" t="str">
         <f t="shared" si="1"/>
@@ -2195,7 +2215,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B117" t="str">
         <f t="shared" si="1"/>
@@ -2207,7 +2227,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B118" t="str">
         <f t="shared" si="1"/>
@@ -2219,7 +2239,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B119" t="str">
         <f t="shared" si="1"/>
@@ -2231,7 +2251,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B120" t="str">
         <f t="shared" si="1"/>
@@ -2243,7 +2263,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B121" t="str">
         <f t="shared" si="1"/>
@@ -2255,7 +2275,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B122" t="str">
         <f t="shared" si="1"/>
@@ -2267,7 +2287,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B123" t="str">
         <f t="shared" si="1"/>
@@ -2279,7 +2299,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B124" t="str">
         <f t="shared" si="1"/>
@@ -2291,7 +2311,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B125" t="str">
         <f t="shared" si="1"/>
@@ -2303,7 +2323,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B126" t="str">
         <f t="shared" si="1"/>
@@ -2315,7 +2335,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B127" t="str">
         <f t="shared" si="1"/>
@@ -2327,7 +2347,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B128" t="str">
         <f t="shared" si="1"/>
@@ -2339,7 +2359,7 @@
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B129" t="str">
         <f t="shared" si="1"/>
@@ -2351,7 +2371,7 @@
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B130" t="str">
         <f t="shared" si="1"/>
@@ -2363,7 +2383,7 @@
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B131" t="str">
         <f t="shared" si="1"/>
@@ -2375,7 +2395,7 @@
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B132" t="str">
         <f t="shared" si="1"/>
@@ -2387,7 +2407,7 @@
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B133" t="str">
         <f t="shared" si="1"/>
@@ -2399,7 +2419,7 @@
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="B134" t="str">
         <f t="shared" si="1"/>
@@ -2409,21 +2429,21 @@
         <v>128</v>
       </c>
       <c r="D134" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E134" s="4"/>
       <c r="F134" s="4"/>
       <c r="G134" s="4"/>
       <c r="P134" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="Q134" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B135" t="str">
         <f t="shared" ref="B135:B198" si="2">DEC2HEX(C135)</f>
@@ -2433,21 +2453,21 @@
         <v>129</v>
       </c>
       <c r="D135" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E135" s="4"/>
       <c r="F135" s="4"/>
       <c r="G135" s="4"/>
       <c r="P135" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="Q135" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="B136" t="str">
         <f t="shared" si="2"/>
@@ -2457,89 +2477,53 @@
         <v>130</v>
       </c>
       <c r="D136" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E136" s="4"/>
       <c r="F136" s="4"/>
       <c r="G136" s="4"/>
       <c r="P136" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="Q136" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>89</v>
-      </c>
-      <c r="B137" t="str">
-        <f t="shared" si="2"/>
-        <v>83</v>
-      </c>
-      <c r="C137">
-        <v>131</v>
-      </c>
-      <c r="D137" s="4" t="s">
-        <v>81</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D137" s="4"/>
       <c r="E137" s="4"/>
       <c r="P137" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q137" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>90</v>
-      </c>
-      <c r="B138" t="str">
-        <f t="shared" si="2"/>
-        <v>84</v>
-      </c>
-      <c r="C138">
-        <v>132</v>
-      </c>
-      <c r="D138" s="4" t="s">
-        <v>81</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D138" s="4"/>
       <c r="E138" s="4"/>
       <c r="P138" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q138" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>12</v>
-      </c>
-      <c r="B139" t="str">
-        <f t="shared" si="2"/>
-        <v>85</v>
-      </c>
-      <c r="C139">
-        <v>133</v>
-      </c>
-      <c r="D139" s="4" t="s">
-        <v>66</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D139" s="4"/>
       <c r="E139" s="4"/>
       <c r="F139" s="4"/>
       <c r="G139" s="4"/>
       <c r="P139" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q139" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="B140" t="str">
         <f t="shared" si="2"/>
@@ -2549,33 +2533,33 @@
         <v>134</v>
       </c>
       <c r="D140" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E140" s="4"/>
       <c r="F140" s="4"/>
       <c r="G140" s="4"/>
       <c r="H140" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I140" s="4"/>
       <c r="J140" s="4"/>
       <c r="K140" s="4"/>
       <c r="L140" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M140" s="4"/>
       <c r="N140" s="4"/>
       <c r="O140" s="4"/>
       <c r="P140" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="Q140" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B141" t="str">
         <f t="shared" si="2"/>
@@ -2587,7 +2571,7 @@
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B142" t="str">
         <f t="shared" si="2"/>
@@ -2599,7 +2583,7 @@
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B143" t="str">
         <f t="shared" si="2"/>
@@ -2611,7 +2595,7 @@
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B144" t="str">
         <f t="shared" si="2"/>
@@ -2623,7 +2607,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B145" t="str">
         <f t="shared" si="2"/>
@@ -2635,7 +2619,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B146" t="str">
         <f t="shared" si="2"/>
@@ -2647,7 +2631,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B147" t="str">
         <f t="shared" si="2"/>
@@ -2659,7 +2643,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B148" t="str">
         <f t="shared" si="2"/>
@@ -2671,7 +2655,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B149" t="str">
         <f t="shared" si="2"/>
@@ -2683,7 +2667,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B150" t="str">
         <f t="shared" si="2"/>
@@ -2695,7 +2679,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B151" t="str">
         <f t="shared" si="2"/>
@@ -2707,7 +2691,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B152" t="str">
         <f t="shared" si="2"/>
@@ -2719,7 +2703,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B153" t="str">
         <f t="shared" si="2"/>
@@ -2731,7 +2715,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B154" t="str">
         <f t="shared" si="2"/>
@@ -2743,7 +2727,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B155" t="str">
         <f t="shared" si="2"/>
@@ -2755,7 +2739,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B156" t="str">
         <f t="shared" si="2"/>
@@ -2767,7 +2751,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B157" t="str">
         <f t="shared" si="2"/>
@@ -2779,7 +2763,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B158" t="str">
         <f t="shared" si="2"/>
@@ -2791,7 +2775,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B159" t="str">
         <f t="shared" si="2"/>
@@ -2803,7 +2787,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B160" t="str">
         <f t="shared" si="2"/>
@@ -2815,7 +2799,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B161" t="str">
         <f t="shared" si="2"/>
@@ -2827,7 +2811,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B162" t="str">
         <f t="shared" si="2"/>
@@ -2839,7 +2823,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B163" t="str">
         <f t="shared" si="2"/>
@@ -2851,7 +2835,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B164" t="str">
         <f t="shared" si="2"/>
@@ -2863,7 +2847,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B165" t="str">
         <f t="shared" si="2"/>
@@ -2875,7 +2859,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B166" t="str">
         <f t="shared" si="2"/>
@@ -2887,7 +2871,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B167" t="str">
         <f t="shared" si="2"/>
@@ -2899,7 +2883,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B168" t="str">
         <f t="shared" si="2"/>
@@ -2911,7 +2895,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B169" t="str">
         <f t="shared" si="2"/>
@@ -2923,7 +2907,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B170" t="str">
         <f t="shared" si="2"/>
@@ -2935,7 +2919,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B171" t="str">
         <f t="shared" si="2"/>
@@ -2947,7 +2931,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B172" t="str">
         <f t="shared" si="2"/>
@@ -2959,7 +2943,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B173" t="str">
         <f t="shared" si="2"/>
@@ -2971,7 +2955,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B174" t="str">
         <f t="shared" si="2"/>
@@ -2983,7 +2967,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B175" t="str">
         <f t="shared" si="2"/>
@@ -2995,7 +2979,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B176" t="str">
         <f t="shared" si="2"/>
@@ -3007,7 +2991,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B177" t="str">
         <f t="shared" si="2"/>
@@ -3019,7 +3003,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B178" t="str">
         <f t="shared" si="2"/>
@@ -3031,7 +3015,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B179" t="str">
         <f t="shared" si="2"/>
@@ -3043,7 +3027,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B180" t="str">
         <f t="shared" si="2"/>
@@ -3055,7 +3039,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B181" t="str">
         <f t="shared" si="2"/>
@@ -3067,7 +3051,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B182" t="str">
         <f t="shared" si="2"/>
@@ -3079,7 +3063,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B183" t="str">
         <f t="shared" si="2"/>
@@ -3091,7 +3075,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B184" t="str">
         <f t="shared" si="2"/>
@@ -3103,7 +3087,7 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B185" t="str">
         <f t="shared" si="2"/>
@@ -3115,7 +3099,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B186" t="str">
         <f t="shared" si="2"/>
@@ -3127,7 +3111,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B187" t="str">
         <f t="shared" si="2"/>
@@ -3139,7 +3123,7 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B188" t="str">
         <f t="shared" si="2"/>
@@ -3151,7 +3135,7 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B189" t="str">
         <f t="shared" si="2"/>
@@ -3163,7 +3147,7 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B190" t="str">
         <f t="shared" si="2"/>
@@ -3175,7 +3159,7 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B191" t="str">
         <f t="shared" si="2"/>
@@ -3187,7 +3171,7 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B192" t="str">
         <f t="shared" si="2"/>
@@ -3199,7 +3183,7 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B193" t="str">
         <f t="shared" si="2"/>
@@ -3211,7 +3195,7 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B194" t="str">
         <f t="shared" si="2"/>
@@ -3223,7 +3207,7 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B195" t="str">
         <f t="shared" si="2"/>
@@ -3235,7 +3219,7 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B196" t="str">
         <f t="shared" si="2"/>
@@ -3247,7 +3231,7 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B197" t="str">
         <f t="shared" si="2"/>
@@ -3259,7 +3243,7 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B198" t="str">
         <f t="shared" si="2"/>
@@ -3271,7 +3255,7 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B199" t="str">
         <f t="shared" ref="B199:B261" si="3">DEC2HEX(C199)</f>
@@ -3283,7 +3267,7 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B200" t="str">
         <f t="shared" si="3"/>
@@ -3295,7 +3279,7 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B201" t="str">
         <f t="shared" si="3"/>
@@ -3307,7 +3291,7 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B202" t="str">
         <f t="shared" si="3"/>
@@ -3319,7 +3303,7 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B203" t="str">
         <f t="shared" si="3"/>
@@ -3331,7 +3315,7 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B204" t="str">
         <f t="shared" si="3"/>
@@ -3343,7 +3327,7 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B205" t="str">
         <f t="shared" si="3"/>
@@ -3355,7 +3339,7 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B206" t="str">
         <f t="shared" si="3"/>
@@ -3367,7 +3351,7 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B207" t="str">
         <f t="shared" si="3"/>
@@ -3379,7 +3363,7 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B208" t="str">
         <f t="shared" si="3"/>
@@ -3391,7 +3375,7 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B209" t="str">
         <f t="shared" si="3"/>
@@ -3403,7 +3387,7 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B210" t="str">
         <f t="shared" si="3"/>
@@ -3415,7 +3399,7 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B211" t="str">
         <f t="shared" si="3"/>
@@ -3427,7 +3411,7 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B212" t="str">
         <f t="shared" si="3"/>
@@ -3439,7 +3423,7 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B213" t="str">
         <f t="shared" si="3"/>
@@ -3451,7 +3435,7 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B214" t="str">
         <f t="shared" si="3"/>
@@ -3463,7 +3447,7 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B215" t="str">
         <f t="shared" si="3"/>
@@ -3475,7 +3459,7 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B216" t="str">
         <f t="shared" si="3"/>
@@ -3487,7 +3471,7 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B217" t="str">
         <f t="shared" si="3"/>
@@ -3499,7 +3483,7 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B218" t="str">
         <f t="shared" si="3"/>
@@ -3511,7 +3495,7 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B219" t="str">
         <f t="shared" si="3"/>
@@ -3523,7 +3507,7 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B220" t="str">
         <f t="shared" si="3"/>
@@ -3535,7 +3519,7 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B221" t="str">
         <f t="shared" si="3"/>
@@ -3547,7 +3531,7 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B222" t="str">
         <f t="shared" si="3"/>
@@ -3559,7 +3543,7 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B223" t="str">
         <f t="shared" si="3"/>
@@ -3571,7 +3555,7 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B224" t="str">
         <f t="shared" si="3"/>
@@ -3583,7 +3567,7 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B225" t="str">
         <f t="shared" si="3"/>
@@ -3595,7 +3579,7 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B226" t="str">
         <f t="shared" si="3"/>
@@ -3607,7 +3591,7 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B227" t="str">
         <f t="shared" si="3"/>
@@ -3619,7 +3603,7 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B228" t="str">
         <f t="shared" si="3"/>
@@ -3631,7 +3615,7 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B229" t="str">
         <f t="shared" si="3"/>
@@ -3643,7 +3627,7 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B230" t="str">
         <f t="shared" si="3"/>
@@ -3655,7 +3639,7 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B231" t="str">
         <f t="shared" si="3"/>
@@ -3667,7 +3651,7 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B232" t="str">
         <f t="shared" si="3"/>
@@ -3679,7 +3663,7 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B233" t="str">
         <f t="shared" si="3"/>
@@ -3691,7 +3675,7 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B234" t="str">
         <f t="shared" si="3"/>
@@ -3703,7 +3687,7 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B235" t="str">
         <f t="shared" si="3"/>
@@ -3715,7 +3699,7 @@
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B236" t="str">
         <f t="shared" si="3"/>
@@ -3727,7 +3711,7 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B237" t="str">
         <f t="shared" si="3"/>
@@ -3739,7 +3723,7 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B238" t="str">
         <f t="shared" si="3"/>
@@ -3751,7 +3735,7 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B239" t="str">
         <f t="shared" si="3"/>
@@ -3763,7 +3747,7 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B240" t="str">
         <f t="shared" si="3"/>
@@ -3775,7 +3759,7 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B241" t="str">
         <f t="shared" si="3"/>
@@ -3787,7 +3771,7 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B242" t="str">
         <f t="shared" si="3"/>
@@ -3799,7 +3783,7 @@
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B243" t="str">
         <f t="shared" si="3"/>
@@ -3811,7 +3795,7 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B244" t="str">
         <f t="shared" si="3"/>
@@ -3823,7 +3807,7 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B245" t="str">
         <f t="shared" si="3"/>
@@ -3835,7 +3819,7 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B246" t="str">
         <f t="shared" si="3"/>
@@ -3847,7 +3831,7 @@
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B247" t="str">
         <f t="shared" si="3"/>
@@ -3859,7 +3843,7 @@
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B248" t="str">
         <f t="shared" si="3"/>
@@ -3871,7 +3855,7 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B249" t="str">
         <f t="shared" si="3"/>
@@ -3883,7 +3867,7 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B250" t="str">
         <f t="shared" si="3"/>
@@ -3895,7 +3879,7 @@
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B251" t="str">
         <f t="shared" si="3"/>
@@ -3907,7 +3891,7 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B252" t="str">
         <f t="shared" si="3"/>
@@ -3919,7 +3903,7 @@
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B253" t="str">
         <f t="shared" si="3"/>
@@ -3931,7 +3915,7 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B254" t="str">
         <f t="shared" si="3"/>
@@ -3943,7 +3927,7 @@
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B255" t="str">
         <f t="shared" si="3"/>
@@ -3955,7 +3939,7 @@
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B256" t="str">
         <f t="shared" si="3"/>
@@ -3967,7 +3951,7 @@
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B257" t="str">
         <f t="shared" si="3"/>
@@ -3979,7 +3963,7 @@
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B258" t="str">
         <f t="shared" si="3"/>
@@ -3991,7 +3975,7 @@
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B259" t="str">
         <f t="shared" si="3"/>
@@ -4003,7 +3987,7 @@
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B260" t="str">
         <f t="shared" si="3"/>
@@ -4015,7 +3999,7 @@
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B261" t="str">
         <f t="shared" si="3"/>
@@ -4026,7 +4010,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="14">
     <mergeCell ref="L140:O140"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="D134:G134"/>
@@ -4037,6 +4021,10 @@
     <mergeCell ref="H140:K140"/>
     <mergeCell ref="D137:E137"/>
     <mergeCell ref="D138:E138"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="H17:K17"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="H18:K18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4044,10 +4032,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1F5E4D-12FB-C749-8B73-7BB9522DEC8B}">
-  <dimension ref="A4:AC13"/>
+  <dimension ref="A4:AC15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4077,224 +4065,243 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" t="s">
         <v>14</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>15</v>
       </c>
-      <c r="M4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4" t="s">
-        <v>17</v>
-      </c>
       <c r="O4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P4" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q4" t="s">
         <v>22</v>
       </c>
-      <c r="P4" t="s">
+      <c r="R4" t="s">
         <v>23</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="S4" t="s">
         <v>24</v>
       </c>
-      <c r="R4" t="s">
+      <c r="T4" t="s">
         <v>25</v>
       </c>
-      <c r="S4" t="s">
+      <c r="U4" t="s">
         <v>26</v>
       </c>
-      <c r="T4" t="s">
+      <c r="V4" t="s">
+        <v>50</v>
+      </c>
+      <c r="W4" t="s">
+        <v>51</v>
+      </c>
+      <c r="X4" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC4" t="s">
         <v>27</v>
-      </c>
-      <c r="U4" t="s">
-        <v>28</v>
-      </c>
-      <c r="V4" t="s">
-        <v>62</v>
-      </c>
-      <c r="W4" t="s">
-        <v>63</v>
-      </c>
-      <c r="X4" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>19</v>
+        <v>2</v>
+      </c>
+      <c r="J6" s="3">
+        <v>1</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="AB6" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J7" t="s">
-        <v>19</v>
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="AB7" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="J8" t="s">
-        <v>19</v>
+        <v>4</v>
+      </c>
+      <c r="J8">
+        <v>3</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="AB8" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="AC8" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="J9" t="s">
-        <v>19</v>
+        <v>5</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="AB9" s="2" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="AC9" s="2" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="J10" t="s">
-        <v>19</v>
+        <v>6</v>
+      </c>
+      <c r="J10">
+        <v>5</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="AB10" s="2" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="AC10" s="2" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="J11" t="s">
-        <v>19</v>
+        <v>7</v>
+      </c>
+      <c r="J11">
+        <v>6</v>
       </c>
       <c r="K11" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="AB11" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="J12" t="s">
         <v>19</v>
       </c>
+      <c r="J12">
+        <v>8</v>
+      </c>
       <c r="K12" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
       <c r="S12" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="T12" s="4"/>
       <c r="U12" s="4"/>
       <c r="V12" s="4"/>
       <c r="W12" s="4" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
       <c r="Z12" s="4"/>
       <c r="AB12" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>92</v>
-      </c>
-      <c r="J13" t="s">
-        <v>19</v>
+        <v>77</v>
+      </c>
+      <c r="J13">
+        <v>9</v>
       </c>
       <c r="K13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N13" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="AB13" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
+      <c r="J14">
+        <v>11</v>
+      </c>
+      <c r="AB14" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>96</v>
+      </c>
+      <c r="J15">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>